<commit_message>
2 entries on RS_Bestellung.csv had wrong validity
</commit_message>
<xml_diff>
--- a/Roadshow/Tag 2/_Testdatengenerator_RS2.xlsx
+++ b/Roadshow/Tag 2/_Testdatengenerator_RS2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://m2datade-my.sharepoint.com/personal/michael_m2data_de/Documents/Dokumente/GitHub/Willibald-Data/Roadshow/Tag 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="400" documentId="8_{651BA3F1-E220-4D83-AC4D-C50AF32EE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2A11BA-83F7-467E-A818-E64A182E4475}"/>
+  <xr:revisionPtr revIDLastSave="403" documentId="8_{651BA3F1-E220-4D83-AC4D-C50AF32EE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{391D95A7-8FCB-4CBE-843F-EB7B2B92A670}"/>
   <bookViews>
-    <workbookView xWindow="2988" yWindow="1236" windowWidth="32220" windowHeight="22884" xr2:uid="{A4E0496F-7324-4B6A-8D8A-BAA11DC38CD8}"/>
+    <workbookView xWindow="3696" yWindow="48" windowWidth="28776" windowHeight="24708" xr2:uid="{A4E0496F-7324-4B6A-8D8A-BAA11DC38CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4585" uniqueCount="1503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="1503">
   <si>
     <t>BestellungID</t>
   </si>
@@ -4583,12 +4583,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -4905,8 +4906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42710005-8F53-432E-93B4-A4A73C28AA15}">
   <dimension ref="A1:N1279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1201" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K1263"/>
+    <sheetView tabSelected="1" topLeftCell="L859" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153:F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9749,8 +9750,8 @@
       <c r="E153" t="s">
         <v>1191</v>
       </c>
-      <c r="F153" s="4">
-        <v>45200</v>
+      <c r="F153" s="5" t="s">
+        <v>1363</v>
       </c>
       <c r="G153" t="s">
         <v>1048</v>
@@ -9792,8 +9793,8 @@
       <c r="E154" t="s">
         <v>1191</v>
       </c>
-      <c r="F154" s="4">
-        <v>45200</v>
+      <c r="F154" s="5" t="s">
+        <v>1363</v>
       </c>
       <c r="G154" t="s">
         <v>1048</v>

</xml_diff>